<commit_message>
renamed Subnets to Subnetwork in the example spreadhsheet
</commit_message>
<xml_diff>
--- a/examples/Rapha_Racing_UAT_Imp_Doc_V2.xlsx
+++ b/examples/Rapha_Racing_UAT_Imp_Doc_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sksa1846/Documents/Projects/Current/TERRAFORM/Rapha Race/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://raxglobal-my.sharepoint.com/personal/carlo_taguinod_rackspace_com/Documents/0-Projects/SANDBOX/rax-apj-build-tool/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB1480A-8C0A-8849-84BF-DC5A77340ED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{0DB1480A-8C0A-8849-84BF-DC5A77340ED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5532F787-38F3-AF4C-B82F-BD81E3099AB9}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="792" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36100" yWindow="3260" windowWidth="28800" windowHeight="16700" tabRatio="792" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="327">
   <si>
     <t xml:space="preserve">Account </t>
   </si>
@@ -1173,6 +1173,9 @@
     <t>- Iremove MS-SQL EC2 instance.
 - Add RDS
 - Setup SG for RDS</t>
+  </si>
+  <si>
+    <t>Subnetworks</t>
   </si>
 </sst>
 </file>
@@ -1503,56 +1506,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="70">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="68">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1592,6 +1546,39 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2081,33 +2068,33 @@
   </dxfs>
   <tableStyles count="4" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
     <tableStyle name="ResourceTables" pivot="0" count="4" xr9:uid="{A25F718D-4690-5F47-8EF4-A305DC474467}">
-      <tableStyleElement type="wholeTable" dxfId="69"/>
-      <tableStyleElement type="headerRow" dxfId="68"/>
-      <tableStyleElement type="firstColumn" dxfId="67"/>
-      <tableStyleElement type="secondRowStripe" dxfId="66"/>
+      <tableStyleElement type="wholeTable" dxfId="67"/>
+      <tableStyleElement type="headerRow" dxfId="66"/>
+      <tableStyleElement type="firstColumn" dxfId="65"/>
+      <tableStyleElement type="secondRowStripe" dxfId="64"/>
     </tableStyle>
     <tableStyle name="SummaryTables" pivot="0" count="3" xr9:uid="{0FC9D21F-78DE-FA4D-9FEC-838D055016BE}">
-      <tableStyleElement type="wholeTable" dxfId="65"/>
-      <tableStyleElement type="headerRow" dxfId="64"/>
-      <tableStyleElement type="firstColumn" dxfId="63"/>
+      <tableStyleElement type="wholeTable" dxfId="63"/>
+      <tableStyleElement type="headerRow" dxfId="62"/>
+      <tableStyleElement type="firstColumn" dxfId="61"/>
     </tableStyle>
     <tableStyle name="TableStyleMedium3 Red" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="62"/>
-      <tableStyleElement type="headerRow" dxfId="61"/>
-      <tableStyleElement type="totalRow" dxfId="60"/>
-      <tableStyleElement type="firstColumn" dxfId="59"/>
-      <tableStyleElement type="lastColumn" dxfId="58"/>
-      <tableStyleElement type="firstRowStripe" dxfId="57"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="56"/>
+      <tableStyleElement type="wholeTable" dxfId="60"/>
+      <tableStyleElement type="headerRow" dxfId="59"/>
+      <tableStyleElement type="totalRow" dxfId="58"/>
+      <tableStyleElement type="firstColumn" dxfId="57"/>
+      <tableStyleElement type="lastColumn" dxfId="56"/>
+      <tableStyleElement type="firstRowStripe" dxfId="55"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="54"/>
     </tableStyle>
     <tableStyle name="TableStyleMedium3 Red Heading" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="55"/>
-      <tableStyleElement type="headerRow" dxfId="54"/>
-      <tableStyleElement type="totalRow" dxfId="53"/>
-      <tableStyleElement type="firstColumn" dxfId="52"/>
-      <tableStyleElement type="lastColumn" dxfId="51"/>
-      <tableStyleElement type="firstRowStripe" dxfId="50"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="49"/>
+      <tableStyleElement type="wholeTable" dxfId="53"/>
+      <tableStyleElement type="headerRow" dxfId="52"/>
+      <tableStyleElement type="totalRow" dxfId="51"/>
+      <tableStyleElement type="firstColumn" dxfId="50"/>
+      <tableStyleElement type="lastColumn" dxfId="49"/>
+      <tableStyleElement type="firstRowStripe" dxfId="48"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="47"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2212,7 +2199,7 @@
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{011A2B45-958B-4922-A984-E636001FF0C6}" name="Global Tags" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{011A2B45-958B-4922-A984-E636001FF0C6}" name="Global Tags" dataDxfId="44"/>
     <tableColumn id="2" xr3:uid="{E60F43DC-153D-4FEC-A43F-D4AF26437688}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="ResourceTables" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2223,8 +2210,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="ALBs" displayName="ALBs" ref="B56:D66" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Application Load Balancers" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="ext-alb" dataDxfId="45" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{A71475A5-C9F4-2742-90C7-2119535FCBAA}" name="int-alb" dataDxfId="44" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="ext-alb" dataDxfId="43" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{A71475A5-C9F4-2742-90C7-2119535FCBAA}" name="int-alb" dataDxfId="42" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="ResourceTables" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2234,13 +2221,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Instances" displayName="Instances" ref="B17:I30" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="EC2 Standalone Instances" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name=" uat-hybris-fe-001" dataDxfId="43" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{53398216-2C62-6C40-AFC2-3833758ADD29}" name=" uat-hybris-fe-002" dataDxfId="42" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{A4D0E3B1-9B92-C541-A4DA-7D47EC3C5806}" name="uat-hybris-sf-001" dataDxfId="41" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{B1A6A669-DBC3-2740-84D5-FB462BBBC8BA}" name="uat-hybris-sf-002" dataDxfId="40" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{A8FCD9C4-C3BA-144A-8376-04C151C626C7}" name=" uat-solr-master" dataDxfId="39" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{891A1DD5-DBDC-3049-883A-F234353B4EC1}" name=" uat-solr-slave" dataDxfId="38" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{4B7A1F70-69B7-074F-8456-978B042898FA}" name="uat-sftp" dataDxfId="37" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name=" uat-hybris-fe-001" dataDxfId="41" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{53398216-2C62-6C40-AFC2-3833758ADD29}" name=" uat-hybris-fe-002" dataDxfId="40" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{A4D0E3B1-9B92-C541-A4DA-7D47EC3C5806}" name="uat-hybris-sf-001" dataDxfId="39" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{B1A6A669-DBC3-2740-84D5-FB462BBBC8BA}" name="uat-hybris-sf-002" dataDxfId="38" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{A8FCD9C4-C3BA-144A-8376-04C151C626C7}" name=" uat-solr-master" dataDxfId="37" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{891A1DD5-DBDC-3049-883A-F234353B4EC1}" name=" uat-solr-slave" dataDxfId="36" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{4B7A1F70-69B7-074F-8456-978B042898FA}" name="uat-sftp" dataDxfId="35" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="ResourceTables" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2250,9 +2237,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="ASGs" displayName="ASGs" ref="B2:E15" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="EC2 Autoscaling Groups" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="uat-admin-fe" dataDxfId="36" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name=" uat-admin-be" dataDxfId="35" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{0FAF9E7B-4C32-AF4C-B9EF-3B13545D510B}" name="uat-solr-slave" dataDxfId="34" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="uat-admin-fe" dataDxfId="34" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name=" uat-admin-be" dataDxfId="33" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{0FAF9E7B-4C32-AF4C-B9EF-3B13545D510B}" name="uat-solr-slave" dataDxfId="32" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="ResourceTables" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2261,8 +2248,8 @@
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="51" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="EFS" displayName="EFS" ref="B97:C103" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="EFS" dataDxfId="33" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="uat-efs" dataDxfId="32" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="EFS" dataDxfId="31" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="uat-efs" dataDxfId="30" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="ResourceTables" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2271,39 +2258,39 @@
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="50" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="S3Buckets" displayName="S3Buckets" ref="B87:C95" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="S3 Buckets / Glacier" dataDxfId="31" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="436185664504-deployment-uat-eu-west-1" dataDxfId="30" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="S3 Buckets / Glacier" dataDxfId="29" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="436185664504-deployment-uat-eu-west-1" dataDxfId="28" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="ResourceTables" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="TargetGroups" displayName="TargetGroups" ref="B69:J76" totalsRowShown="0" tableBorderDxfId="29" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="TargetGroups" displayName="TargetGroups" ref="B69:J76" totalsRowShown="0" tableBorderDxfId="27" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="Target Groups" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="ext-alb-80-tg" dataDxfId="28" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{122BC03E-8BC2-495A-87BD-6F1B8C4C4CA2}" name="ext-alb-443-tg" dataDxfId="27" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{29E0B7B8-5F75-A545-8485-D9796580CD99}" name="int-alb-tg" dataDxfId="26" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{8A1AED87-5064-6B42-8970-83AEFFCF9BFF}" name="ext-nlb-tg" dataDxfId="25" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{353A6E9D-71EC-244C-A6B8-7282C902C883}" name="int-nlb-hybris-80-tg" dataDxfId="24" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{0551727B-5057-A24F-AEDA-C2A2A130FDA4}" name="int-nlb-hybris-8009-tg" dataDxfId="23" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{1FC8F478-1FFF-FD4D-A0A1-716FC105BEFC}" name="int-nlb-admin-be-80-tg" dataDxfId="22" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{A80B6924-4C08-9A4F-BA8C-E9D85738BC8D}" name="int-nlb-admin-be-8009-tg" dataDxfId="21" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="ext-alb-80-tg" dataDxfId="26" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{122BC03E-8BC2-495A-87BD-6F1B8C4C4CA2}" name="ext-alb-443-tg" dataDxfId="25" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{29E0B7B8-5F75-A545-8485-D9796580CD99}" name="int-alb-tg" dataDxfId="24" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{8A1AED87-5064-6B42-8970-83AEFFCF9BFF}" name="ext-nlb-tg" dataDxfId="23" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{353A6E9D-71EC-244C-A6B8-7282C902C883}" name="int-nlb-hybris-80-tg" dataDxfId="22" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{0551727B-5057-A24F-AEDA-C2A2A130FDA4}" name="int-nlb-hybris-8009-tg" dataDxfId="21" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{1FC8F478-1FFF-FD4D-A0A1-716FC105BEFC}" name="int-nlb-admin-be-80-tg" dataDxfId="20" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{A80B6924-4C08-9A4F-BA8C-E9D85738BC8D}" name="int-nlb-admin-be-8009-tg" dataDxfId="19" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="ResourceTables" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{02B819BA-6C5F-214F-AB5C-5EFAD585ABA4}" name="NLBs" displayName="NLBs" ref="B47:G54" totalsRowShown="0" tableBorderDxfId="20" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{02B819BA-6C5F-214F-AB5C-5EFAD585ABA4}" name="NLBs" displayName="NLBs" ref="B47:G54" totalsRowShown="0" tableBorderDxfId="18" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{C696D916-6AD4-A349-84AB-4569BD2FB83D}" name="Network Load Balancers" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{B2DFAF86-6BBA-B049-BA36-DC5C204FC0C9}" name="ext-nlb" dataDxfId="19" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{B2DFAF86-6BBA-B049-BA36-DC5C204FC0C9}" name="ext-nlb" dataDxfId="17" dataCellStyle="Normal"/>
     <tableColumn id="3" xr3:uid="{FCB31860-8AF0-3349-928A-54ECE448AD0A}" name="int-nlb-hybris" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{A44CB625-E238-A745-9E0E-FAABFFE6FAC3}" name="int-nlb-admin" dataDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{D06BDBC6-3BBA-4049-B404-8D2B6DA1309A}" name="int-nlbsolr-m" dataDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{F67189B2-7C1F-B940-939E-422587490661}" name="int-nlbsolr-_x000a_s" dataDxfId="16" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{A44CB625-E238-A745-9E0E-FAABFFE6FAC3}" name="int-nlb-admin" dataDxfId="16" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{D06BDBC6-3BBA-4049-B404-8D2B6DA1309A}" name="int-nlbsolr-m" dataDxfId="15" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{F67189B2-7C1F-B940-939E-422587490661}" name="int-nlbsolr-_x000a_s" dataDxfId="14" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="ResourceTables" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2313,7 +2300,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="56" xr:uid="{00000000-000C-0000-FFFF-FFFF1A000000}" name="ElasticacheRedis" displayName="ElasticacheRedis" ref="B17:C34" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-1A00-000001000000}" name="Elasticache - Redis" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1A00-000002000000}" name="uat-redis" dataDxfId="15" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1A00-000002000000}" name="uat-redis" dataDxfId="13" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="ResourceTables" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2334,10 +2321,10 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{5221A530-5119-5F4E-A251-587909B0B3CB}" name="RDS" displayName="RDS" ref="B2:C15" totalsRowShown="0" dataDxfId="3" tableBorderDxfId="2" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{5221A530-5119-5F4E-A251-587909B0B3CB}" name="RDS" displayName="RDS" ref="B2:C15" totalsRowShown="0" dataDxfId="12" tableBorderDxfId="11" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3171D40D-348B-E24D-AA0D-818E3822F058}" name="RDS" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{5DB2E6C0-E45B-274F-A3CD-B284826DF06D}" name="ProdRds" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{3171D40D-348B-E24D-AA0D-818E3822F058}" name="RDS" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{5DB2E6C0-E45B-274F-A3CD-B284826DF06D}" name="ProdRds" dataDxfId="9" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="ResourceTables" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2370,7 +2357,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C2BDCC7D-EDE7-824F-83FD-5EE622BDD2E7}" name="IAM Resource Name"/>
     <tableColumn id="2" xr3:uid="{7ED06237-8FF2-3B4B-86A6-9E5D0434C143}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{71B3E827-94DF-7E48-B355-8FF1D3C78DD1}" name="Access to Services" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{71B3E827-94DF-7E48-B355-8FF1D3C78DD1}" name="Access to Services" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{935E7066-3487-2948-A5BF-8E51CC2BFB9D}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="ResourceTables" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2378,7 +2365,7 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{CD9DD177-93DA-460F-B401-9B9E10C1A1EC}" name="CodeDeployApp" displayName="CodeDeployApp" ref="B2:E5" totalsRowShown="0" tableBorderDxfId="13" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{CD9DD177-93DA-460F-B401-9B9E10C1A1EC}" name="CodeDeployApp" displayName="CodeDeployApp" ref="B2:E5" totalsRowShown="0" tableBorderDxfId="7" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="B2:E5" xr:uid="{5522AB56-B4A2-4615-BD0E-67FEBE87F08C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2387,16 +2374,16 @@
   </autoFilter>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{101A6E50-7913-43BB-A013-588C23355545}" name="CodeDeploy Applications" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{A004D697-4657-4A43-AAFE-E23741B3DB67}" name="uat-fe" dataDxfId="12" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{A633B7E6-825D-714D-8A2E-8AED22EC08FD}" name="uat-be" dataDxfId="11" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{96BC0C79-828E-3946-9EDD-4027658A624E}" name="uat-solv" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{A004D697-4657-4A43-AAFE-E23741B3DB67}" name="uat-fe" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{A633B7E6-825D-714D-8A2E-8AED22EC08FD}" name="uat-be" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{96BC0C79-828E-3946-9EDD-4027658A624E}" name="uat-solv" dataDxfId="4" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="ResourceTables" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{77DF0F01-972A-468D-BF52-FB313847A9B2}" name="CodeDeployDeployments" displayName="CodeDeployDeployments" ref="B7:E15" totalsRowShown="0" tableBorderDxfId="9" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{77DF0F01-972A-468D-BF52-FB313847A9B2}" name="CodeDeployDeployments" displayName="CodeDeployDeployments" ref="B7:E15" totalsRowShown="0" tableBorderDxfId="3" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="B7:E15" xr:uid="{1C6492C8-E2EB-41AD-BEC3-79F84492DC7B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2405,9 +2392,9 @@
   </autoFilter>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B004DB86-F6BD-4385-B304-926FDAC11AF0}" name="CodeDeploy Deployments" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{222304CE-A7CF-4579-8AAA-25B3C8E5D4D5}" name="fedeployment" dataDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{3732C63B-71DA-4845-AA56-FFA9F98B3BBA}" name="bedeployment" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{9B47FB94-94A4-8142-B7C4-05A89A407C2A}" name="solvdeployment" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{222304CE-A7CF-4579-8AAA-25B3C8E5D4D5}" name="fedeployment" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{3732C63B-71DA-4845-AA56-FFA9F98B3BBA}" name="bedeployment" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{9B47FB94-94A4-8142-B7C4-05A89A407C2A}" name="solvdeployment" dataDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="ResourceTables" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2438,7 +2425,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="VPC" displayName="VPC" ref="B5:C13" totalsRowShown="0" tableBorderDxfId="48" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="VPC" displayName="VPC" ref="B5:C13" totalsRowShown="0" tableBorderDxfId="46" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="B5:C13" xr:uid="{00000000-0009-0000-0100-000004000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2452,9 +2439,9 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Subnets" displayName="Subnets" ref="B15:F19" totalsRowShown="0" tableBorderDxfId="47" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Subnets" displayName="Subnets" ref="B15:F19" totalsRowShown="0" tableBorderDxfId="45" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Subnets" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Subnetworks" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Public-AZ1" dataCellStyle="Normal"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Public-AZ2" dataCellStyle="Normal"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Private-AZ1" dataCellStyle="Normal"/>
@@ -2946,7 +2933,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:F48"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3050,7 +3039,7 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>26</v>
+        <v>326</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
@@ -5280,7 +5269,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>136</v>
       </c>
@@ -6816,7 +6805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:E15"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7036,15 +7025,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100115BDFBCBC55954DBE3A036F43C688BE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2602281623a1436ad7b29323987829d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6be0c7cb-7b3c-42ff-aba9-440d72149579" xmlns:ns3="de305a12-becf-467d-a6c1-7efafa548d98" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6563a88de22b55a81dac40f5abe7b9cd" ns2:_="" ns3:_="">
     <xsd:import namespace="6be0c7cb-7b3c-42ff-aba9-440d72149579"/>
@@ -7223,6 +7203,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7230,14 +7219,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67FBEE8F-C278-44E2-AAC4-E0F2E05597DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3E69D3C-B089-40EA-8109-45FCB7B3FCBC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7256,19 +7237,27 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67FBEE8F-C278-44E2-AAC4-E0F2E05597DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34B1892E-3E6C-4CE1-BBE1-31A16A61250C}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="de305a12-becf-467d-a6c1-7efafa548d98"/>
+    <ds:schemaRef ds:uri="6be0c7cb-7b3c-42ff-aba9-440d72149579"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6be0c7cb-7b3c-42ff-aba9-440d72149579"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="de305a12-becf-467d-a6c1-7efafa548d98"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>